<commit_message>
CalorimeterV4 update 2.2 isort
</commit_message>
<xml_diff>
--- a/strategy_ocae.xlsx
+++ b/strategy_ocae.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,32 +671,122 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>T_r3</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>T_r4</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>T_r5</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>T_A</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>T_B</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>T_out</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>U_pre</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>U_r1</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>U_r2</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>U_r3</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>U_r4</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>U_r5</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>PWM_pre</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>PWM_r1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>PWM_r2</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>PWM_r3</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>PWM_r4</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>PWM_r5</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mW_pre</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mW_r1</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>mW_r2</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>mW_r3</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mW_r4</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>mW_r5</t>
         </is>
       </c>
     </row>

</xml_diff>